<commit_message>
II da IV pasuxebi
</commit_message>
<xml_diff>
--- a/PhysicsExperiments.xlsx
+++ b/PhysicsExperiments.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabak\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\PhysicsMechanics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F14ECE-5328-4D16-99A2-C73268A2DA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88491C1-B6CB-4DD1-B0DF-73423F459662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02603006-0041-44C1-99BD-A7230703DB2F}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>σ =</t>
   </si>
@@ -607,9 +607,6 @@
     <t>60 გრამი</t>
   </si>
   <si>
-    <t>75 გრამი</t>
-  </si>
-  <si>
     <r>
       <t>აჩქარება
 (მ/წმ</t>
@@ -749,18 +746,128 @@
       <t xml:space="preserve"> - σ =</t>
     </r>
   </si>
+  <si>
+    <t>70 გრამი</t>
+  </si>
+  <si>
+    <t xml:space="preserve">პასუხები:
+1) მაქსიმალურად შევამციროთ ცდომილება.
+საწყისი სიჩქარე უნდა იყოს 0;
+2) წინაღობის შედეგად აჩქარება შემცირდება;
+</t>
+  </si>
+  <si>
+    <t>3) როცა წინაღობის ძალა g-ს გაუტოლდება;
+4) ერთდროულად;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">პასუხები:
+1) აშკარად ჩანს;
+2) ექსპერიმენტის ცდომილება არ აღემატება 0.1%-ს;
+3) არ შეიცვლება ხახუნის კოეფიციენტი,  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">mg sinα = µmg cosα;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4) ამის შედეგად ცდომილება გაიზრდება;
+5) µ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> არის მაქსიმალური მნიშვნელობა, µ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt; µ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;
+6) კი, როდესაც 2 სხეულის ზედაპირი თითქმის იდეალურად ბრტყელია/გაპრიალებულია, ხახუნის კოეფიციენტი ბევრად აღემატება 1-ს;</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -845,13 +952,6 @@
     <font>
       <vertAlign val="superscript"/>
       <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1041,7 +1141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1070,15 +1170,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1091,26 +1182,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1147,6 +1241,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3495,15 +3622,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>371474</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3526,6 +3653,252 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>16946</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88E035FC-FE1F-43AD-B71E-E8BB8D1C97D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5503346" y="1619251"/>
+          <a:ext cx="1478479" cy="1457324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>579782</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28147</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38F35EF5-54CC-4841-9186-01A5F3909147}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7065893" y="1578665"/>
+          <a:ext cx="1481759" cy="1514047"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>97047</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>118613</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>539151</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>370216</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AA48A39-1936-4E1A-9C25-B28CF8C3F39F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5596387" y="1660585"/>
+          <a:ext cx="1053141" cy="251603"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ka-GE" sz="800"/>
+            <a:t>წინაღობის</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ka-GE" sz="800" baseline="0"/>
+            <a:t> გარეშე</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>452887</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>111424</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>327085</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE313892-8F01-4399-BCAF-889E5759AB16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7174302" y="1653396"/>
+          <a:ext cx="769189" cy="215661"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ka-GE" sz="800"/>
+            <a:t>წინაღობით</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3590,12 +3963,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>409812</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1132618" cy="396327"/>
+    <xdr:ext cx="1017843" cy="396327"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
@@ -3609,8 +3982,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="552450" y="4152900"/>
-          <a:ext cx="1132618" cy="396327"/>
+          <a:off x="7182087" y="1009650"/>
+          <a:ext cx="1017843" cy="396327"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3653,8 +4026,12 @@
             <a:t>F</a:t>
           </a:r>
           <a:r>
+            <a:rPr lang="ka-GE" sz="1800" baseline="-25000"/>
+            <a:t>ხახ</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="ka-GE" sz="1800"/>
-            <a:t>ხახ = µ</a:t>
+            <a:t> = µ</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1800"/>
@@ -3667,10 +4044,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>438150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1114425" cy="428625"/>
     <xdr:sp macro="" textlink="">
@@ -3686,7 +4063,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="514349" y="4772025"/>
+          <a:off x="7115174" y="1438275"/>
           <a:ext cx="1114425" cy="428625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3796,16 +4173,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>285749</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>638175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3820,8 +4197,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1904999" y="4181475"/>
-          <a:ext cx="2790825" cy="447675"/>
+          <a:off x="6362700" y="2371725"/>
+          <a:ext cx="2657476" cy="457200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3859,7 +4236,15 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1800"/>
-            <a:t>Fmax = mg sin</a:t>
+            <a:t>F</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="30000"/>
+            <a:t>max</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t> = mg sin</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="el-GR" sz="1800"/>
@@ -3881,16 +4266,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>904875</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>533400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3905,7 +4290,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1933575" y="4791075"/>
+          <a:off x="6838950" y="1905000"/>
           <a:ext cx="1600200" cy="361950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3944,7 +4329,15 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1800"/>
-            <a:t>ma = mg - µkN</a:t>
+            <a:t>ma = mg - µ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="-25000"/>
+            <a:t>k</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>N</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4264,21 +4657,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.35">
@@ -4366,11 +4759,11 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="8"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="36">
+      <c r="K6" s="29"/>
+      <c r="L6" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="31">
         <f>(M3+M4)</f>
         <v>2.1579990564646669</v>
       </c>
@@ -4387,8 +4780,8 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
-      <c r="L7" s="37" t="s">
-        <v>41</v>
+      <c r="L7" s="32" t="s">
+        <v>40</v>
       </c>
       <c r="M7" s="4">
         <f>(M3*M4)</f>
@@ -4465,10 +4858,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1AF488-8A07-44F3-B45D-4ED1CA3499D8}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4477,22 +4870,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
     </row>
     <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
@@ -4519,6 +4912,13 @@
       <c r="I3" s="17" t="s">
         <v>22</v>
       </c>
+      <c r="J3" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
     </row>
     <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
@@ -4548,6 +4948,11 @@
       <c r="I4" s="1">
         <v>9.7893340000000002</v>
       </c>
+      <c r="J4" s="57"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -4577,6 +4982,11 @@
       <c r="I5" s="1">
         <v>9.8269470000000005</v>
       </c>
+      <c r="J5" s="57"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -4606,6 +5016,11 @@
       <c r="I6" s="1">
         <v>9.811223</v>
       </c>
+      <c r="J6" s="57"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -4635,6 +5050,11 @@
       <c r="I7" s="1">
         <v>9.8327930000000006</v>
       </c>
+      <c r="J7" s="55"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
     </row>
     <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -4664,59 +5084,90 @@
       <c r="I8" s="1">
         <v>9.774661</v>
       </c>
+      <c r="J8" s="56"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
     </row>
-    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
+    </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K11" s="38" t="s">
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="40"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="38"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K12" s="41"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="43"/>
+    <row r="15" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="39"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="41"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K13" s="41"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="43"/>
+    <row r="16" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="39"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="41"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K14" s="41"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="43"/>
+    <row r="17" spans="10:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="44"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K15" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="45"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="46"/>
+    <row r="18" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J18" s="42"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="44"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K16" s="44"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="46"/>
+    <row r="19" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J19" s="42"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="44"/>
     </row>
-    <row r="17" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K17" s="47"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="49"/>
+    <row r="20" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J20" s="45"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
+    <mergeCell ref="J9:N11"/>
+    <mergeCell ref="J14:M16"/>
+    <mergeCell ref="J17:M20"/>
     <mergeCell ref="A1:N1"/>
-    <mergeCell ref="K11:N14"/>
-    <mergeCell ref="K15:N17"/>
+    <mergeCell ref="J3:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -4735,22 +5186,22 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4764,36 +5215,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9539C81-82B6-45CB-A056-2EC90B7C30A0}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="7" width="15.140625" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
     </row>
     <row r="4" spans="1:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -4807,109 +5259,233 @@
         <v>29</v>
       </c>
       <c r="F4" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>33</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="23">
-        <v>1.3472999999999999</v>
-      </c>
-      <c r="D5" s="23">
-        <v>1.3469</v>
-      </c>
-      <c r="E5" s="23">
-        <v>1.329</v>
-      </c>
-      <c r="F5" s="23">
+      <c r="C5" s="20">
+        <v>1.4676</v>
+      </c>
+      <c r="D5" s="20">
+        <v>1.4705999999999999</v>
+      </c>
+      <c r="E5" s="20">
+        <v>1.4693000000000001</v>
+      </c>
+      <c r="F5" s="20">
         <v>0.556917</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="20">
         <v>0.40139000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="20">
         <v>0.96840000000000004</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="20">
         <v>0.97640000000000005</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="20">
         <v>0.97009999999999996</v>
       </c>
-      <c r="F6" s="23">
-        <v>0.16281200000000001</v>
-      </c>
-      <c r="G6" s="23">
+      <c r="F6" s="20">
+        <v>1.0628120000000001</v>
+      </c>
+      <c r="G6" s="20">
         <v>0.40792</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="23">
+      <c r="B7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="20">
         <v>0.7984</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="21">
         <v>0.80100000000000005</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="20">
         <v>0.79679999999999995</v>
       </c>
-      <c r="F7" s="23">
-        <v>0.15625</v>
-      </c>
-      <c r="G7" s="23">
+      <c r="F7" s="50">
+        <v>1.5625</v>
+      </c>
+      <c r="G7" s="20">
         <v>0.40544999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I8" s="6"/>
+      <c r="J8" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I9" s="12"/>
+      <c r="J9" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23"/>
+      <c r="I10" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="49"/>
+      <c r="K10" s="24">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="51"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H13" s="6"/>
-      <c r="I13" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" s="28" t="s">
-        <v>36</v>
-      </c>
+      <c r="A13" s="51"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H14" s="12"/>
-      <c r="I14" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="J14" s="29" t="s">
-        <v>38</v>
-      </c>
+      <c r="A14" s="51"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
     </row>
-    <row r="17" spans="8:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="33"/>
-      <c r="J17" s="27">
-        <v>1E-3</v>
-      </c>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="51"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="51"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="51"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="51"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="51"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="H17:I17"/>
+  <mergeCells count="3">
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A11:L19"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
meotxe eqsperimenthsi mesame pasuxi shevasworet
</commit_message>
<xml_diff>
--- a/PhysicsExperiments.xlsx
+++ b/PhysicsExperiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\PhysicsMechanics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0F4D5E-91FF-4B7A-9010-BB700849B7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE06502-3D77-491C-9AF3-E4FB0DB42977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{02603006-0041-44C1-99BD-A7230703DB2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02603006-0041-44C1-99BD-A7230703DB2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment_1" sheetId="1" r:id="rId1"/>
@@ -762,6 +762,478 @@
   </si>
   <si>
     <r>
+      <t>ცდა 1
+t</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (წმ)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ცდა 2
+t</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (წმ)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ცდა 3
+t</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (წმ)</t>
+    </r>
+  </si>
+  <si>
+    <t>20-900
+(გრ)</t>
+  </si>
+  <si>
+    <t>40-880
+(გრ)</t>
+  </si>
+  <si>
+    <t>4-1840
+(გრ)</t>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <t>0.4 მ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D = </t>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1თეორიული</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <r>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2თეორიული</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3თეორიული</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">პასუხები:
 1) აშკარად ჩანს;
 2) ექსპერიმენტის ცდომილება არ აღემატება 0.1%-ს;
@@ -776,7 +1248,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">mg sinα = µmg cosα;
+      <t xml:space="preserve">f(x) = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µmg</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">;
 </t>
     </r>
     <r>
@@ -853,478 +1346,6 @@
       </rPr>
       <t>;
 6) კი, როდესაც 2 სხეულის ზედაპირი თითქმის იდეალურად ბრტყელია/გაპრიალებულია, ხახუნის კოეფიციენტი ბევრად აღემატება 1-ს;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ცდა 1
-t</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (წმ)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ცდა 2
-t</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (წმ)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ცდა 3
-t</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (წმ)</t>
-    </r>
-  </si>
-  <si>
-    <t>20-900
-(გრ)</t>
-  </si>
-  <si>
-    <t>40-880
-(გრ)</t>
-  </si>
-  <si>
-    <t>4-1840
-(გრ)</t>
-  </si>
-  <si>
-    <r>
-      <t>M</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>M</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>H</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>M</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>M</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>F</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>M</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <t>0.4 მ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D = </t>
-  </si>
-  <si>
-    <r>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1თეორიული</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>t</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>II</t>
-  </si>
-  <si>
-    <t>III</t>
-  </si>
-  <si>
-    <r>
-      <t>t</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>t</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2თეორიული</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3თეორიული</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =</t>
     </r>
   </si>
 </sst>
@@ -1339,7 +1360,7 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1467,6 +1488,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1686,6 +1714,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1743,6 +1788,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1751,29 +1802,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5196,7 +5224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4EFAF04-10AE-472A-9F56-F1601CEB5CA6}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -5207,21 +5235,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
     </row>
     <row r="2" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -5419,22 +5447,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
     </row>
     <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
@@ -5461,13 +5489,13 @@
       <c r="I3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="53" t="s">
+      <c r="J3" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
     </row>
     <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
@@ -5497,11 +5525,11 @@
       <c r="I4" s="1">
         <v>9.7893340000000002</v>
       </c>
-      <c r="J4" s="53"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -5531,11 +5559,11 @@
       <c r="I5" s="1">
         <v>9.8269470000000005</v>
       </c>
-      <c r="J5" s="53"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -5565,11 +5593,11 @@
       <c r="I6" s="1">
         <v>9.811223</v>
       </c>
-      <c r="J6" s="53"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -5640,75 +5668,75 @@
       <c r="N8" s="33"/>
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J9" s="37" t="s">
+      <c r="J9" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="45"/>
+      <c r="N9" s="45"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="45"/>
+      <c r="N10" s="45"/>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="45"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J14" s="39" t="s">
+      <c r="J14" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="41"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="48"/>
     </row>
     <row r="15" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J15" s="42"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="44"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="51"/>
     </row>
     <row r="16" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J16" s="42"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="44"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="51"/>
     </row>
     <row r="17" spans="10:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J17" s="45" t="s">
+      <c r="J17" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="47"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="54"/>
     </row>
     <row r="18" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J18" s="45"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="47"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="54"/>
     </row>
     <row r="19" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J19" s="45"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="47"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="54"/>
     </row>
     <row r="20" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J20" s="48"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="50"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="56"/>
+      <c r="M20" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5740,54 +5768,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
       <c r="L1" s="21"/>
       <c r="M1" s="21"/>
       <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="60" t="s">
+      <c r="A2" s="37" t="s">
         <v>56</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>55</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="G2" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="64"/>
+      <c r="H2" s="42"/>
       <c r="I2" s="33"/>
       <c r="J2" s="33"/>
       <c r="K2" s="33"/>
     </row>
     <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="61">
+      <c r="A3" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="39">
         <v>0.52</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="18">
         <v>1.6779999999999999</v>
@@ -5804,14 +5832,14 @@
       <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="61">
+      <c r="A4" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="39">
         <v>0.02</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1">
         <v>1.2065999999999999</v>
@@ -5828,14 +5856,14 @@
       <c r="K4" s="33"/>
     </row>
     <row r="5" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="61">
+      <c r="A5" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="39">
         <v>0.92</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="18">
         <v>1.79</v>
@@ -5852,10 +5880,10 @@
       <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="61">
+      <c r="A6" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="39">
         <v>0.36</v>
       </c>
       <c r="H6" s="33"/>
@@ -5864,108 +5892,108 @@
       <c r="K6" s="33"/>
     </row>
     <row r="7" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="61">
+      <c r="A7" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="39">
         <v>0.02</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="63"/>
+      <c r="G7" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="66"/>
-      <c r="G7" s="65" t="s">
+      <c r="H7" s="63"/>
+      <c r="J7" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="66"/>
-      <c r="J7" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="K7" s="66"/>
+      <c r="K7" s="63"/>
     </row>
     <row r="8" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="59" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="61">
+      <c r="A8" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="39">
         <v>1.84</v>
       </c>
-      <c r="D8" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="62">
+      <c r="D8" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="40">
         <v>1.6717</v>
       </c>
-      <c r="G8" s="58" t="s">
+      <c r="G8" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="40">
+        <v>1.2009000000000001</v>
+      </c>
+      <c r="J8" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="62">
-        <v>1.2009000000000001</v>
-      </c>
-      <c r="J8" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="K8" s="62">
+      <c r="K8" s="40">
         <v>1.7833000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="58" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="62">
+      <c r="D9" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="40">
         <v>0.2863</v>
       </c>
-      <c r="G9" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="H9" s="62">
+      <c r="G9" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="40">
         <v>0.55469999999999997</v>
       </c>
-      <c r="J9" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="K9" s="62">
+      <c r="J9" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="40">
         <v>0.25159999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="62">
+      <c r="D10" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="40">
         <v>0.21329999999999999</v>
       </c>
-      <c r="G10" s="58" t="s">
+      <c r="G10" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="40">
+        <v>0.42649999999999999</v>
+      </c>
+      <c r="J10" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="H10" s="62">
-        <v>0.42649999999999999</v>
-      </c>
-      <c r="J10" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="K10" s="62">
+      <c r="K10" s="40">
         <v>0.21329999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="58" t="s">
+      <c r="D11" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="63">
+      <c r="E11" s="41">
         <v>0.34</v>
       </c>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="63">
+      <c r="H11" s="41">
         <v>0.3</v>
       </c>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="K11" s="63">
+      <c r="K11" s="41">
         <v>0.18</v>
       </c>
     </row>
@@ -5988,8 +6016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9539C81-82B6-45CB-A056-2EC90B7C30A0}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6000,20 +6028,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
       <c r="M1" s="21"/>
       <c r="N1" s="21"/>
       <c r="O1" s="21"/>
@@ -6116,141 +6144,141 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22"/>
-      <c r="I10" s="55" t="s">
+      <c r="I10" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="56"/>
+      <c r="J10" s="65"/>
       <c r="K10" s="23">
         <v>1E-3</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
+      <c r="A11" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="57"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="66"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="57"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57"/>
-      <c r="L13" s="57"/>
+      <c r="A13" s="66"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="66"/>
+      <c r="L14" s="66"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="57"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
+      <c r="A15" s="66"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="66"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="57"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="66"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="57"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="66"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="57"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
+      <c r="A18" s="66"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="66"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="57"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
+      <c r="A19" s="66"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
mesame gavaumjobese; mexute gavaswore; meeqvse daviwke;
</commit_message>
<xml_diff>
--- a/PhysicsExperiments.xlsx
+++ b/PhysicsExperiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\PhysicsMechanics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85C2079-E8DC-4D8E-8BED-5B1E5A210B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B51611-4052-42B1-A71D-80918995281F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{02603006-0041-44C1-99BD-A7230703DB2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{02603006-0041-44C1-99BD-A7230703DB2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment_0" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Experiment_3" sheetId="4" r:id="rId4"/>
     <sheet name="Experiment_4" sheetId="5" r:id="rId5"/>
     <sheet name="Experiment_5" sheetId="6" r:id="rId6"/>
+    <sheet name="Experiment_6" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="112">
   <si>
     <t>σ =</t>
   </si>
@@ -508,12 +509,6 @@
 (წმ)</t>
   </si>
   <si>
-    <t>50 გრამი</t>
-  </si>
-  <si>
-    <t>60 გრამი</t>
-  </si>
-  <si>
     <r>
       <t>აჩქარება
 (მ/წმ</t>
@@ -541,9 +536,6 @@
     </r>
   </si>
   <si>
-    <t>საწყისი ოწნა:</t>
-  </si>
-  <si>
     <t>110გრ</t>
   </si>
   <si>
@@ -606,9 +598,6 @@
       </rPr>
       <t xml:space="preserve"> - σ =</t>
     </r>
-  </si>
-  <si>
-    <t>70 გრამი</t>
   </si>
   <si>
     <t xml:space="preserve">პასუხები:
@@ -1141,32 +1130,6 @@
   </si>
   <si>
     <r>
-      <t>F</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>k
-ხახუნის ძალა</t>
-    </r>
-  </si>
-  <si>
-    <t>პასუხები:
-1) აშკარად ჩანს;
-2) ექსპერიმენტის ცდომილება არ აღემატება 0.1%-ს;
-3) არ შეიცვლება ხახუნის კოეფიციენტი,  f(x) = µmg;
-4) ამის შედეგად ცდომილება გაიზრდება;
-5) µs არის მაქსიმალური მნიშვნელობა, µs &gt; µk;
-6) კი, როდესაც 2 სხეულის ზედაპირი თითქმის იდეალურად ბრტყელია/გაპრიალებულია, ხახუნის კოეფიციენტი ბევრად აღემატება 1-ს;</t>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="20"/>
         <color theme="1"/>
@@ -1291,22 +1254,6 @@
     <t>ექსპერიმენტი ციფრული წამზომით</t>
   </si>
   <si>
-    <r>
-      <t>V</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>საშ</t>
-    </r>
-  </si>
-  <si>
     <t>4.992 მ/წმ</t>
   </si>
   <si>
@@ -1316,22 +1263,6 @@
   <si>
     <t>გრადუსი
 θ (დახრა)</t>
-  </si>
-  <si>
-    <r>
-      <t>θ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>საშ</t>
-    </r>
   </si>
   <si>
     <t>5.96°</t>
@@ -1403,30 +1334,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ექსპერიმენტი IV</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-ბალისტიკური ქანქარა</t>
-    </r>
-  </si>
-  <si>
     <t>ექსპერიმენტი ბალისტიკური ქანქარით</t>
   </si>
   <si>
@@ -1496,6 +1403,297 @@
       </rPr>
       <t xml:space="preserve"> =</t>
     </r>
+  </si>
+  <si>
+    <t>ძელაკის წონა</t>
+  </si>
+  <si>
+    <t>კგ</t>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ხახუნის ძალა (ნ)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ურიკისსაწყისი</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> წონა:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>საშ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>θ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>საშ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ექსპერიმენტი V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ბალისტიკური ქანქარა</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ექსპერიმენტი VI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+დრეკადი და არადრეკადი  დაჯახება</t>
+    </r>
+  </si>
+  <si>
+    <t>დრეკადი დაჯახება</t>
+  </si>
+  <si>
+    <t>0.40 მ</t>
+  </si>
+  <si>
+    <t>0.518 კგ</t>
+  </si>
+  <si>
+    <t>6.3 მ/წმ</t>
+  </si>
+  <si>
+    <t>5.7 მ/წმ</t>
+  </si>
+  <si>
+    <t>L =</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>v</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1b </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>v</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <t>დანაკარგი:</t>
+  </si>
+  <si>
+    <t>21.3 მ/წმ</t>
+  </si>
+  <si>
+    <t>16.7 მ/წმ</t>
   </si>
 </sst>
 </file>
@@ -1509,7 +1707,7 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1647,6 +1845,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1656,7 +1861,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1796,11 +2001,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1884,9 +2126,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1903,8 +2142,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1969,26 +2214,56 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4728,7 +5003,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>27546</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>247650</xdr:rowOff>
@@ -4809,7 +5084,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>28574</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>609600</xdr:rowOff>
@@ -4938,16 +5213,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>685800</xdr:rowOff>
+      <xdr:rowOff>542925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4962,8 +5237,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7115175" y="2419350"/>
-          <a:ext cx="2219325" cy="352425"/>
+          <a:off x="7019925" y="2447925"/>
+          <a:ext cx="2362200" cy="352425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5031,16 +5306,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>676275</xdr:rowOff>
+      <xdr:rowOff>514350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5055,8 +5330,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7115175" y="2047875"/>
-          <a:ext cx="1352550" cy="361950"/>
+          <a:off x="7019925" y="2057400"/>
+          <a:ext cx="1495425" cy="361950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5104,6 +5379,137 @@
             <a:rPr lang="en-US" sz="1600"/>
             <a:t>N</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CABDD73F-3801-4DF3-A003-83464EEB694E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28575" y="4410075"/>
+          <a:ext cx="7134225" cy="1847850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ka-GE" sz="1200" b="1"/>
+            <a:t>პასუხები:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ka-GE" sz="1200"/>
+            <a:t>1) აშკარად ჩანს;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ka-GE" sz="1200"/>
+            <a:t>2) ექსპერიმენტის ცდომილება არ აღემატება 0.1%-ს;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ka-GE" sz="1200"/>
+            <a:t>3) არ შეიცვლება ხახუნის კოეფიციენტი,  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>f(x) = µmg;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>4) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ka-GE" sz="1200"/>
+            <a:t>ამის შედეგად ცდომილება გაიზრდება;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ka-GE" sz="1200"/>
+            <a:t>5) µ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>s </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ka-GE" sz="1200"/>
+            <a:t>არის მაქსიმალური მნიშვნელობა, µ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>s &gt; µk;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>6) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ka-GE" sz="1200"/>
+            <a:t>კი, როდესაც 2 სხეულის ზედაპირი თითქმის იდეალურად ბრტყელია/გაპრიალებულია, ხახუნის კოეფიციენტი ბევრად აღემატება 1-ს;</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -6443,15 +6849,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>809625</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>157161</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6466,8 +6872,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2552700" y="3633786"/>
-          <a:ext cx="6210300" cy="2700339"/>
+          <a:off x="2524125" y="3290886"/>
+          <a:ext cx="6210300" cy="2862264"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6546,12 +6952,330 @@
         <a:p>
           <a:r>
             <a:rPr lang="ka-GE" sz="1200" baseline="0"/>
-            <a:t>    ბ) თუ ორივე ფოტორელე აღიქვამს ბურთს და თან ვიცით, რომ თავისუფალი ფრენის დროს ჰორიზონტალური სიჩქარე არ იცვლება, მაშინ გავლენა არ ექვს;</a:t>
+            <a:t>    ბ) თუ ორივე ფოტორელე აღიქვამს ბურთს და თან ვიცით, რომ თავისუფალი ფრენის დროს ჰორიზონტალური სიჩქარე არ იცვლება, მაშინ გავლენა არ აქვს;</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F392C407-A7E4-4E83-9FD7-13FF6D622DBE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5495924" y="1000126"/>
+              <a:ext cx="1981201" cy="514350"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:schemeClr val="dk1"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>დანაკარგი: </m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="|"/>
+                        <m:endChr m:val="|"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:f>
+                          <m:fPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:fPr>
+                          <m:num>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑣</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>2</m:t>
+                                </m:r>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑎</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>−</m:t>
+                            </m:r>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑣</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>1</m:t>
+                                </m:r>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑏</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                          </m:num>
+                          <m:den>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑣</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>1</m:t>
+                                </m:r>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑏</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                          </m:den>
+                        </m:f>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>∗10</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="ka-GE" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>0</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F392C407-A7E4-4E83-9FD7-13FF6D622DBE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5495924" y="1000126"/>
+              <a:ext cx="1981201" cy="514350"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>დანაკარგი: </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>|(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑣_2𝑎−𝑣_1𝑏)/𝑣_1𝑏 |∗10</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>0</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6867,21 +7591,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
+      <c r="A1" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -6970,7 +7694,7 @@
       <c r="H6" s="7"/>
       <c r="K6" s="23"/>
       <c r="L6" s="24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M6" s="25">
         <f>(M3+M4)</f>
@@ -6990,7 +7714,7 @@
       <c r="G7" s="9"/>
       <c r="H7" s="10"/>
       <c r="L7" s="26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M7" s="3">
         <f>(M3*M4)</f>
@@ -7079,22 +7803,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
+      <c r="A1" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
     </row>
     <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
@@ -7121,13 +7845,13 @@
       <c r="I3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="68" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
+      <c r="J3" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
     </row>
     <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
@@ -7157,11 +7881,11 @@
       <c r="I4" s="1">
         <v>9.7893340000000002</v>
       </c>
-      <c r="J4" s="68"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -7191,11 +7915,11 @@
       <c r="I5" s="1">
         <v>9.8269470000000005</v>
       </c>
-      <c r="J5" s="68"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -7225,11 +7949,11 @@
       <c r="I6" s="1">
         <v>9.811223</v>
       </c>
-      <c r="J6" s="68"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -7300,75 +8024,75 @@
       <c r="N8" s="28"/>
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J9" s="52" t="s">
-        <v>63</v>
-      </c>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="53"/>
+      <c r="J9" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="53"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J14" s="54" t="s">
+      <c r="J14" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="57"/>
     </row>
     <row r="15" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J15" s="57"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="58"/>
-      <c r="M15" s="59"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="60"/>
     </row>
     <row r="16" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J16" s="57"/>
-      <c r="K16" s="58"/>
-      <c r="L16" s="58"/>
-      <c r="M16" s="59"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="60"/>
     </row>
     <row r="17" spans="10:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J17" s="60" t="s">
+      <c r="J17" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="63"/>
     </row>
     <row r="18" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J18" s="60"/>
-      <c r="K18" s="61"/>
-      <c r="L18" s="61"/>
-      <c r="M18" s="62"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="62"/>
+      <c r="L18" s="62"/>
+      <c r="M18" s="63"/>
     </row>
     <row r="19" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J19" s="60"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="62"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="63"/>
     </row>
     <row r="20" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J20" s="63"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="65"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -7400,39 +8124,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
+      <c r="A1" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
       <c r="L1" s="21"/>
       <c r="M1" s="21"/>
       <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14" ht="33" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H2" s="36"/>
       <c r="I2" s="28"/>
@@ -7441,13 +8165,13 @@
     </row>
     <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B3" s="33">
         <v>0.52</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E3" s="18">
         <v>1.6779999999999999</v>
@@ -7465,13 +8189,13 @@
     </row>
     <row r="4" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B4" s="33">
         <v>0.02</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E4" s="1">
         <v>1.2065999999999999</v>
@@ -7489,13 +8213,13 @@
     </row>
     <row r="5" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B5" s="33">
         <v>0.92</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E5" s="18">
         <v>1.79</v>
@@ -7513,7 +8237,7 @@
     </row>
     <row r="6" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B6" s="33">
         <v>0.36</v>
@@ -7525,45 +8249,45 @@
     </row>
     <row r="7" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B7" s="33">
         <v>0.02</v>
       </c>
-      <c r="D7" s="70" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="71"/>
-      <c r="G7" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="71"/>
-      <c r="J7" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="K7" s="71"/>
+      <c r="D7" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="72"/>
+      <c r="G7" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="72"/>
+      <c r="J7" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" s="72"/>
     </row>
     <row r="8" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B8" s="33">
         <v>1.84</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E8" s="34">
         <v>1.6717</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H8" s="34">
         <v>1.2009000000000001</v>
       </c>
       <c r="J8" s="37" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="K8" s="34">
         <v>1.7833000000000001</v>
@@ -7571,19 +8295,19 @@
     </row>
     <row r="9" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D9" s="37" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E9" s="34">
         <v>0.2863</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H9" s="34">
         <v>0.55469999999999997</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K9" s="34">
         <v>0.25159999999999999</v>
@@ -7591,19 +8315,19 @@
     </row>
     <row r="10" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D10" s="37" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E10" s="34">
         <v>0.21329999999999999</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H10" s="34">
         <v>0.42649999999999999</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K10" s="34">
         <v>0.21329999999999999</v>
@@ -7611,19 +8335,19 @@
     </row>
     <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="37" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E11" s="35">
         <v>0.34</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H11" s="35">
         <v>0.3</v>
       </c>
       <c r="J11" s="37" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K11" s="35">
         <v>0.18</v>
@@ -7649,306 +8373,323 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0.42578125" customWidth="1"/>
-    <col min="2" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="7" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" customWidth="1"/>
+    <col min="3" max="4" width="6.42578125" customWidth="1"/>
+    <col min="5" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="21"/>
+      <c r="A1" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
       <c r="O1" s="21"/>
       <c r="P1" s="21"/>
     </row>
-    <row r="4" spans="1:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="16" t="s">
+    <row r="4" spans="1:16" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="F4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="G4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="H4" s="38" t="s">
-        <v>65</v>
+      <c r="H4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="19">
+      <c r="B5" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="31">
+        <v>0.05</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="19">
         <v>1.4676</v>
       </c>
-      <c r="D5" s="19">
+      <c r="F5" s="19">
         <v>1.4705999999999999</v>
       </c>
-      <c r="E5" s="19">
+      <c r="G5" s="19">
         <v>1.4693000000000001</v>
       </c>
-      <c r="F5" s="19">
+      <c r="H5" s="19">
         <v>0.556917</v>
       </c>
-      <c r="G5" s="19">
+      <c r="I5" s="19">
         <v>0.40139000000000002</v>
       </c>
-      <c r="H5" s="76">
-        <f>50*9.8*G5</f>
-        <v>196.68110000000004</v>
+      <c r="J5" s="49">
+        <f>(9.80665*C5*I5)</f>
+        <v>0.19681456217500001</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="19">
+      <c r="B6" s="80"/>
+      <c r="C6" s="31">
+        <v>0.06</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="19">
         <v>0.96840000000000004</v>
       </c>
-      <c r="D6" s="19">
+      <c r="F6" s="19">
         <v>0.97640000000000005</v>
       </c>
-      <c r="E6" s="19">
+      <c r="G6" s="19">
         <v>0.97009999999999996</v>
       </c>
-      <c r="F6" s="19">
+      <c r="H6" s="19">
         <v>1.0628120000000001</v>
       </c>
-      <c r="G6" s="19">
+      <c r="I6" s="19">
         <v>0.40792</v>
       </c>
-      <c r="H6" s="76">
-        <f>60*9.8*G6</f>
-        <v>239.85696000000002</v>
+      <c r="J6" s="49">
+        <f t="shared" ref="J6:J7" si="0">(9.80665*C6*I6)</f>
+        <v>0.24001972007999997</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="19">
+      <c r="B7" s="81"/>
+      <c r="C7" s="31">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="19">
         <v>0.7984</v>
       </c>
-      <c r="D7" s="20">
+      <c r="F7" s="20">
         <v>0.80100000000000005</v>
       </c>
-      <c r="E7" s="19">
+      <c r="G7" s="19">
         <v>0.79679999999999995</v>
       </c>
-      <c r="F7" s="27">
+      <c r="H7" s="27">
         <v>1.5625</v>
       </c>
-      <c r="G7" s="19">
+      <c r="I7" s="19">
         <v>0.40544999999999998</v>
       </c>
-      <c r="H7" s="76">
-        <f>70*9.8*G7</f>
-        <v>278.13869999999997</v>
+      <c r="J7" s="49">
+        <f t="shared" si="0"/>
+        <v>0.27832743697500001</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G8" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="H8" s="77">
-        <f>(AVERAGE(H5:H7))</f>
-        <v>238.22558666666669</v>
-      </c>
-      <c r="J8" s="39"/>
-      <c r="K8" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8" s="41" t="s">
-        <v>30</v>
+      <c r="I8" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="50">
+        <f>(AVERAGE(J5:J7))</f>
+        <v>0.23838723974333331</v>
+      </c>
+      <c r="L8" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="M8" s="77"/>
+      <c r="N8" s="41" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J9" s="39"/>
-      <c r="K9" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" s="41" t="s">
-        <v>32</v>
+      <c r="L9" s="39"/>
+      <c r="M9" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="41" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22"/>
-      <c r="J10" s="72" t="s">
-        <v>33</v>
-      </c>
-      <c r="K10" s="73"/>
-      <c r="L10" s="78">
+      <c r="L10" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="79"/>
+      <c r="N10" s="51">
         <v>1E-3</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
-      <c r="B11" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="74"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
       <c r="M11" s="42"/>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
       <c r="M12" s="42"/>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="42"/>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="74"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
       <c r="M13" s="42"/>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="42"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="74"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="74"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
       <c r="M14" s="42"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="42"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="74"/>
-      <c r="J15" s="74"/>
-      <c r="K15" s="74"/>
-      <c r="L15" s="74"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
       <c r="M15" s="42"/>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="42"/>
-      <c r="B16" s="74"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="74"/>
-      <c r="L16" s="74"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
       <c r="M16" s="42"/>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="42"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="74"/>
-      <c r="L17" s="74"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
       <c r="M17" s="42"/>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="42"/>
-      <c r="B18" s="74"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="74"/>
-      <c r="L18" s="74"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
       <c r="M18" s="42"/>
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42"/>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="74"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="74"/>
-      <c r="L19" s="74"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
       <c r="M19" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="B11:L19"/>
-    <mergeCell ref="A1:L1"/>
+  <mergeCells count="4">
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -7967,8 +8708,271 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD34F534-8F62-43AA-9740-81595D0D0225}">
+  <dimension ref="A1:O10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="7.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="21"/>
+    </row>
+    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+    </row>
+    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="44">
+        <v>0.02</v>
+      </c>
+      <c r="F5" s="44">
+        <v>0.02</v>
+      </c>
+      <c r="G5" s="44">
+        <v>0.02</v>
+      </c>
+      <c r="H5" s="44">
+        <v>2.01E-2</v>
+      </c>
+      <c r="I5" s="44">
+        <v>0.02</v>
+      </c>
+      <c r="J5" s="44">
+        <v>2.01E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="45">
+        <v>5</v>
+      </c>
+      <c r="F6" s="45">
+        <v>5</v>
+      </c>
+      <c r="G6" s="45">
+        <v>5</v>
+      </c>
+      <c r="H6" s="45">
+        <v>4.9749999999999996</v>
+      </c>
+      <c r="I6" s="45">
+        <v>5</v>
+      </c>
+      <c r="J6" s="45">
+        <v>4.9749999999999996</v>
+      </c>
+      <c r="L6" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="M6" s="32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D8" s="73" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="E9" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="L10" s="31" t="s">
         <v>97</v>
+      </c>
+      <c r="M10" s="32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D3:J3"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="A1:N1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55D09DC-E39F-4D44-9F38-DC60927FED1E}">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="12.85546875" customWidth="1"/>
+    <col min="6" max="7" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>99</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -7985,229 +8989,123 @@
       <c r="N1" s="67"/>
       <c r="O1" s="67"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H8" t="s">
-        <v>98</v>
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="88" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="89"/>
+      <c r="D4" s="9"/>
+      <c r="F4" s="88" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="89"/>
+    </row>
+    <row r="5" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="83" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="F5" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="83" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="84" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="83" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="F6" s="84" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="83" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="83" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="F7" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="83" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="85" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="86" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="F8" s="85" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="86" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H9" t="s">
-        <v>99</v>
+      <c r="B9" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="87">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="F9" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9" s="87">
+        <v>3.9E-2</v>
       </c>
     </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
-  </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD34F534-8F62-43AA-9740-81595D0D0225}">
-  <dimension ref="A1:O10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="7.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="21"/>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
     </row>
-    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="75" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
     </row>
-    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>78</v>
-      </c>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
-    <row r="5" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="45">
-        <v>0.02</v>
-      </c>
-      <c r="F5" s="45">
-        <v>0.02</v>
-      </c>
-      <c r="G5" s="45">
-        <v>0.02</v>
-      </c>
-      <c r="H5" s="45">
-        <v>2.01E-2</v>
-      </c>
-      <c r="I5" s="45">
-        <v>0.02</v>
-      </c>
-      <c r="J5" s="45">
-        <v>2.01E-2</v>
-      </c>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
-    <row r="6" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" s="46">
-        <v>5</v>
-      </c>
-      <c r="F6" s="46">
-        <v>5</v>
-      </c>
-      <c r="G6" s="46">
-        <v>5</v>
-      </c>
-      <c r="H6" s="46">
-        <v>4.9749999999999996</v>
-      </c>
-      <c r="I6" s="46">
-        <v>5</v>
-      </c>
-      <c r="J6" s="46">
-        <v>4.9749999999999996</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="M6" s="50" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D8" s="75" t="s">
-        <v>96</v>
-      </c>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D9" s="1"/>
-      <c r="E9" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="H9" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="J9" s="44" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="F10" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="H10" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="I10" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="J10" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="L10" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="M10" s="50" t="s">
-        <v>86</v>
-      </c>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D3:J3"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
meotcex morcha. wesit kvela morcha
</commit_message>
<xml_diff>
--- a/PhysicsExperiments.xlsx
+++ b/PhysicsExperiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\PhysicsMechanics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC934D6-DE8B-484B-8D20-26C18EA269E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D40161-AE1D-4E38-BEEF-C8D178DEA826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="4" xr2:uid="{02603006-0041-44C1-99BD-A7230703DB2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{02603006-0041-44C1-99BD-A7230703DB2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment_0" sheetId="1" r:id="rId1"/>
@@ -2500,6 +2500,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2592,26 +2612,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5870,16 +5870,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>257176</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -5896,8 +5896,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3867150" y="2009775"/>
-              <a:ext cx="3781425" cy="495300"/>
+              <a:off x="619126" y="2676525"/>
+              <a:ext cx="3600450" cy="495300"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5940,7 +5940,9 @@
                   <m:f>
                     <m:fPr>
                       <m:ctrlPr>
-                        <a:rPr lang="ka-GE" sz="1600" i="1"/>
+                        <a:rPr lang="ka-GE" sz="1600" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
                       </m:ctrlPr>
                     </m:fPr>
                     <m:num>
@@ -5949,7 +5951,9 @@
                           <m:begChr m:val="|"/>
                           <m:endChr m:val="|"/>
                           <m:ctrlPr>
-                            <a:rPr lang="ka-GE" sz="1600" i="1"/>
+                            <a:rPr lang="ka-GE" sz="1600" i="1">
+                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            </a:rPr>
                           </m:ctrlPr>
                         </m:dPr>
                         <m:e>
@@ -6029,8 +6033,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3867150" y="2009775"/>
-              <a:ext cx="3781425" cy="495300"/>
+              <a:off x="619126" y="2676525"/>
+              <a:ext cx="3600450" cy="495300"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6076,13 +6080,13 @@
                 <a:rPr lang="en-US" sz="1600" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑀𝑔−𝐹_𝑐</a:t>
+                <a:t>𝑀𝑔−𝐹_𝑐 |</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="ka-GE" sz="1600" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t> |/</a:t>
+                <a:t>/</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1600" b="0" i="0">
@@ -6091,6 +6095,1018 @@
                 <a:t>𝑀𝑔∗100%=6.1%</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A89A56CA-4A0B-402E-8F04-393DAE2725D5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="276225" y="3571876"/>
+              <a:ext cx="8648700" cy="2324100"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="1"/>
+                <a:t>პასუხები:</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="1"/>
+                <a:t>1)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" baseline="0"/>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>აჩერებს დედამიწის მიზიდულობის ძალა. თუ ეს ძალა გაქრება მაშინ თანამგზავრები ღია კოსმოსში გაიფანტებიან;</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>2) </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>ცენტრისკენული აჩქარება მაქსიმალური იქნება ეკვატორის ხაზთან, ხოლო მინიმალური პოლუსებთან, რადგან </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>a=wR w - </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>არის კუთხური სიჩქარე და ის დედამიწის ნებისმიერ წერტილში ერთიდაიგივეა ხოლო ბრუნვის ღერძამდე მანძილი ეკვატორთან არის ყველაზე დიდი;</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>3)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> ალასკაში აწონილი ოქრო მცირედით მძიმე იქნება, რადგან უფრო ახლოსაა დედამიწის ბრუნვის ღერძთან და ცენტრისკენული აჩქარება უფრო ნაკლებია;</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>4)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>იმიტომ რომ ჩამოსრიალებისას მიენიჭება არამხოლოდ </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>x</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>,</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>არამედ </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>y </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>სიჩქარეც, იმისთვის რომ შეეხოს იმ წერტილს რომელიც მდებარეობს გზის შუაში, </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>x </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>სიჩქარე უნდა იყოს ნული;</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>5)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>𝑎</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>= </m:t>
+                  </m:r>
+                  <m:f>
+                    <m:fPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="dk1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:fPr>
+                    <m:num>
+                      <m:sSup>
+                        <m:sSupPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="dk1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="+mn-lt"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSupPr>
+                        <m:e>
+                          <m:r>
+                            <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="dk1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="+mn-lt"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>𝑣</m:t>
+                          </m:r>
+                        </m:e>
+                        <m:sup>
+                          <m:r>
+                            <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="dk1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="+mn-lt"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>2</m:t>
+                          </m:r>
+                        </m:sup>
+                      </m:sSup>
+                    </m:num>
+                    <m:den>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="dk1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝑟</m:t>
+                      </m:r>
+                    </m:den>
+                  </m:f>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>→10= </m:t>
+                  </m:r>
+                  <m:f>
+                    <m:fPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="dk1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:fPr>
+                    <m:num>
+                      <m:sSup>
+                        <m:sSupPr>
+                          <m:ctrlPr>
+                            <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="dk1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="+mn-lt"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                          </m:ctrlPr>
+                        </m:sSupPr>
+                        <m:e>
+                          <m:r>
+                            <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="dk1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="+mn-lt"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>𝑣</m:t>
+                          </m:r>
+                        </m:e>
+                        <m:sup>
+                          <m:r>
+                            <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                              <a:solidFill>
+                                <a:schemeClr val="dk1"/>
+                              </a:solidFill>
+                              <a:effectLst/>
+                              <a:latin typeface="+mn-lt"/>
+                              <a:ea typeface="+mn-ea"/>
+                              <a:cs typeface="+mn-cs"/>
+                            </a:rPr>
+                            <m:t>2</m:t>
+                          </m:r>
+                        </m:sup>
+                      </m:sSup>
+                    </m:num>
+                    <m:den>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="dk1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>20</m:t>
+                      </m:r>
+                    </m:den>
+                  </m:f>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>→</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>𝑣</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>=</m:t>
+                  </m:r>
+                  <m:rad>
+                    <m:radPr>
+                      <m:degHide m:val="on"/>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="dk1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:radPr>
+                    <m:deg/>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="dk1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>200</m:t>
+                      </m:r>
+                    </m:e>
+                  </m:rad>
+                </m:oMath>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A89A56CA-4A0B-402E-8F04-393DAE2725D5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="276225" y="3571876"/>
+              <a:ext cx="8648700" cy="2324100"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="9525" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="1"/>
+                <a:t>პასუხები:</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="1"/>
+                <a:t>1)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" baseline="0"/>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>აჩერებს დედამიწის მიზიდულობის ძალა. თუ ეს ძალა გაქრება მაშინ თანამგზავრები ღია კოსმოსში გაიფანტებიან;</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>2) </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>ცენტრისკენული აჩქარება მაქსიმალური იქნება ეკვატორის ხაზთან, ხოლო მინიმალური პოლუსებთან, რადგან </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>a=wR w - </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>არის კუთხური სიჩქარე და ის დედამიწის ნებისმიერ წერტილში ერთიდაიგივეა ხოლო ბრუნვის ღერძამდე მანძილი ეკვატორთან არის ყველაზე დიდი;</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>3)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> ალასკაში აწონილი ოქრო მცირედით მძიმე იქნება, რადგან უფრო ახლოსაა დედამიწის ბრუნვის ღერძთან და ცენტრისკენული აჩქარება უფრო ნაკლებია;</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>4)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>იმიტომ რომ ჩამოსრიალებისას მიენიჭება არამხოლოდ </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>x</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>,</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>არამედ </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>y </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>სიჩქარეც, იმისთვის რომ შეეხოს იმ წერტილს რომელიც მდებარეობს გზის შუაში, </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>x </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>სიჩქარე უნდა იყოს ნული;</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="1" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>5)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ka-GE" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑎= </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> 𝑣^2</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>/𝑟</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>→10= </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> 𝑣^2/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>20</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>→𝑣=√200</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1200" b="1"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -8336,21 +9352,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
     </row>
     <row r="2" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -8548,22 +9564,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
     </row>
     <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
@@ -8590,13 +9606,13 @@
       <c r="I3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="79" t="s">
+      <c r="J3" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
+      <c r="M3" s="88"/>
+      <c r="N3" s="88"/>
     </row>
     <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
@@ -8626,11 +9642,11 @@
       <c r="I4" s="1">
         <v>9.7893340000000002</v>
       </c>
-      <c r="J4" s="79"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -8660,11 +9676,11 @@
       <c r="I5" s="1">
         <v>9.8269470000000005</v>
       </c>
-      <c r="J5" s="79"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="80"/>
-      <c r="M5" s="80"/>
-      <c r="N5" s="80"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="88"/>
+      <c r="M5" s="88"/>
+      <c r="N5" s="88"/>
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -8694,11 +9710,11 @@
       <c r="I6" s="1">
         <v>9.811223</v>
       </c>
-      <c r="J6" s="79"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="80"/>
-      <c r="M6" s="80"/>
-      <c r="N6" s="80"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="88"/>
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -8769,75 +9785,75 @@
       <c r="N8" s="28"/>
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J9" s="63" t="s">
+      <c r="J9" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="64"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="72"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="64"/>
-      <c r="N10" s="64"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="72"/>
+      <c r="N10" s="72"/>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J11" s="64"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="64"/>
-      <c r="N11" s="64"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="72"/>
+      <c r="N11" s="72"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J14" s="65" t="s">
+      <c r="J14" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="K14" s="66"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="67"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="75"/>
     </row>
     <row r="15" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J15" s="68"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="70"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="77"/>
+      <c r="M15" s="78"/>
     </row>
     <row r="16" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J16" s="68"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="70"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="77"/>
+      <c r="L16" s="77"/>
+      <c r="M16" s="78"/>
     </row>
     <row r="17" spans="10:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J17" s="71" t="s">
+      <c r="J17" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="72"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="73"/>
+      <c r="K17" s="80"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="81"/>
     </row>
     <row r="18" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J18" s="71"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="72"/>
-      <c r="M18" s="73"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="80"/>
+      <c r="L18" s="80"/>
+      <c r="M18" s="81"/>
     </row>
     <row r="19" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J19" s="71"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="73"/>
+      <c r="J19" s="79"/>
+      <c r="K19" s="80"/>
+      <c r="L19" s="80"/>
+      <c r="M19" s="81"/>
     </row>
     <row r="20" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J20" s="74"/>
-      <c r="K20" s="75"/>
-      <c r="L20" s="75"/>
-      <c r="M20" s="76"/>
+      <c r="J20" s="82"/>
+      <c r="K20" s="83"/>
+      <c r="L20" s="83"/>
+      <c r="M20" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -8869,19 +9885,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
       <c r="L1" s="21"/>
       <c r="M1" s="21"/>
       <c r="N1" s="21"/>
@@ -8999,18 +10015,18 @@
       <c r="B7" s="33">
         <v>0.02</v>
       </c>
-      <c r="D7" s="81" t="s">
+      <c r="D7" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="82"/>
-      <c r="G7" s="81" t="s">
+      <c r="E7" s="90"/>
+      <c r="G7" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="82"/>
-      <c r="J7" s="81" t="s">
+      <c r="H7" s="90"/>
+      <c r="J7" s="89" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="82"/>
+      <c r="K7" s="90"/>
     </row>
     <row r="8" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="31" t="s">
@@ -9133,22 +10149,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
       <c r="O1" s="21"/>
       <c r="P1" s="21"/>
     </row>
@@ -9175,7 +10191,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="95" t="s">
         <v>89</v>
       </c>
       <c r="C5" s="31">
@@ -9205,7 +10221,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="88"/>
+      <c r="B6" s="96"/>
       <c r="C6" s="31">
         <v>0.06</v>
       </c>
@@ -9233,7 +10249,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="89"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="31">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -9268,10 +10284,10 @@
         <f>(AVERAGE(J5:J7))</f>
         <v>0.23838723974333331</v>
       </c>
-      <c r="L8" s="85" t="s">
+      <c r="L8" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="M8" s="86"/>
+      <c r="M8" s="94"/>
       <c r="N8" s="41" t="s">
         <v>27</v>
       </c>
@@ -9287,10 +10303,10 @@
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22"/>
-      <c r="L10" s="83" t="s">
+      <c r="L10" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="M10" s="84"/>
+      <c r="M10" s="92"/>
       <c r="N10" s="51">
         <v>1E-3</v>
       </c>
@@ -9445,177 +10461,170 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1606FDA-2A00-4E45-A273-11FFE99BEEE9}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="7" width="12.5703125" customWidth="1"/>
+    <col min="2" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" customWidth="1"/>
     <col min="9" max="10" width="9.85546875" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="21" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="85" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="99" t="s">
+    <row r="3" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="62" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="63" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="63" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="62">
+        <v>1</v>
+      </c>
+      <c r="B4" s="62">
+        <v>0.12</v>
+      </c>
+      <c r="C4" s="62">
+        <v>7.06</v>
+      </c>
+      <c r="D4" s="64">
+        <v>6.86</v>
+      </c>
+      <c r="E4" s="64">
+        <v>7.43</v>
+      </c>
+      <c r="F4" s="65">
+        <f>(AVERAGE(C4:E4))</f>
+        <v>7.1166666666666671</v>
+      </c>
+      <c r="G4" s="62">
+        <v>0.51</v>
+      </c>
+      <c r="I4" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="J4" s="34" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="99" t="s">
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="62">
+        <v>2</v>
+      </c>
+      <c r="B5" s="62">
+        <v>0.15</v>
+      </c>
+      <c r="C5" s="65">
+        <v>7.5</v>
+      </c>
+      <c r="D5" s="64">
+        <v>8.35</v>
+      </c>
+      <c r="E5" s="64">
+        <v>7.75</v>
+      </c>
+      <c r="F5" s="65">
+        <f t="shared" ref="F5:F6" si="0">(AVERAGE(C5:E5))</f>
+        <v>7.8666666666666671</v>
+      </c>
+      <c r="G5" s="62">
+        <v>0.52</v>
+      </c>
+      <c r="I5" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="J5" s="34" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="99" t="s">
+    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="62">
+        <v>3</v>
+      </c>
+      <c r="B6" s="62">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="62">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="D6" s="62">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="E6" s="65">
+        <v>8.9</v>
+      </c>
+      <c r="F6" s="65">
+        <f t="shared" si="0"/>
+        <v>8.9666666666666668</v>
+      </c>
+      <c r="G6" s="62">
+        <v>0.54</v>
+      </c>
+      <c r="I6" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="J6" s="34" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="99" t="s">
+    <row r="7" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="66"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="G7" s="67" t="s">
+        <v>131</v>
+      </c>
+      <c r="I7" s="68" t="s">
         <v>123</v>
       </c>
-      <c r="C11" s="100">
+      <c r="J7" s="69">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="93" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" s="94" t="s">
-        <v>127</v>
-      </c>
-      <c r="D15" s="94" t="s">
-        <v>128</v>
-      </c>
-      <c r="E15" s="94" t="s">
-        <v>129</v>
-      </c>
-      <c r="F15" s="94" t="s">
-        <v>130</v>
-      </c>
-      <c r="G15" s="94" t="s">
-        <v>125</v>
-      </c>
-      <c r="H15" s="94" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="93">
-        <v>1</v>
-      </c>
-      <c r="C16" s="93">
-        <v>0.12</v>
-      </c>
-      <c r="D16" s="93">
-        <v>7.06</v>
-      </c>
-      <c r="E16" s="95">
-        <v>6.86</v>
-      </c>
-      <c r="F16" s="95">
-        <v>7.43</v>
-      </c>
-      <c r="G16" s="96">
-        <f>(AVERAGE(D16:F16))</f>
-        <v>7.1166666666666671</v>
-      </c>
-      <c r="H16" s="93">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="93">
-        <v>2</v>
-      </c>
-      <c r="C17" s="93">
-        <v>0.15</v>
-      </c>
-      <c r="D17" s="96">
-        <v>7.5</v>
-      </c>
-      <c r="E17" s="95">
-        <v>8.35</v>
-      </c>
-      <c r="F17" s="95">
-        <v>7.75</v>
-      </c>
-      <c r="G17" s="96">
-        <f t="shared" ref="G17:G18" si="0">(AVERAGE(D17:F17))</f>
-        <v>7.8666666666666671</v>
-      </c>
-      <c r="H17" s="93">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="93">
-        <v>3</v>
-      </c>
-      <c r="C18" s="93">
-        <v>0.2</v>
-      </c>
-      <c r="D18" s="93">
-        <v>9.0500000000000007</v>
-      </c>
-      <c r="E18" s="93">
-        <v>8.9499999999999993</v>
-      </c>
-      <c r="F18" s="96">
-        <v>8.9</v>
-      </c>
-      <c r="G18" s="96">
-        <f t="shared" si="0"/>
-        <v>8.9666666666666668</v>
-      </c>
-      <c r="H18" s="93">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B19" s="97"/>
-      <c r="C19" s="97"/>
-      <c r="D19" s="97"/>
-      <c r="E19" s="97"/>
-      <c r="F19" s="97"/>
-      <c r="G19" s="54" t="s">
-        <v>132</v>
-      </c>
-      <c r="H19" s="98" t="s">
-        <v>131</v>
-      </c>
-    </row>
+    <row r="15" spans="1:10" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
@@ -9643,22 +10652,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="85" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
       <c r="O1" s="21"/>
     </row>
     <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.35">
@@ -9668,15 +10677,15 @@
       <c r="B3" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="90" t="s">
+      <c r="D3" s="98" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
     </row>
     <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="47" t="s">
@@ -9764,15 +10773,15 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D8" s="90" t="s">
+      <c r="D8" s="98" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="98"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="98"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
@@ -9857,15 +10866,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="85" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
       <c r="H1" s="61"/>
       <c r="I1" s="61"/>
       <c r="J1" s="61"/>
@@ -9876,14 +10885,14 @@
       <c r="O1" s="61"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="92"/>
-      <c r="E3" s="91" t="s">
+      <c r="C3" s="100"/>
+      <c r="E3" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="92"/>
+      <c r="F3" s="100"/>
     </row>
     <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B4" s="31" t="s">

</xml_diff>